<commit_message>
Sabtu 08 November 2025 19.05 WIB
</commit_message>
<xml_diff>
--- a/ORG/RAB LKKMD 2025 FIKS.xlsx
+++ b/ORG/RAB LKKMD 2025 FIKS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Himatif\RAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tisa\Tisa\ORG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A335C285-7B76-4E58-9339-6705789724CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACFCE8-57DE-4F12-8725-21958B84B33F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,8 +251,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$Rp-3809]* #,##0_-;\-[$Rp-3809]* #,##0_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$Rp-3809]* #,##0_-;\-[$Rp-3809]* #,##0_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -487,19 +487,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,25 +508,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -541,10 +541,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,6 +556,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -568,86 +634,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,8 +973,8 @@
   </sheetPr>
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="79" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="41" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1001,80 +1001,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47" t="s">
+      <c r="E5" s="49"/>
+      <c r="F5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="54" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="52"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="55"/>
     </row>
     <row r="7" spans="2:9" s="3" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
@@ -1083,9 +1083,9 @@
       <c r="C7" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="24">
         <f>SUM(G8)</f>
         <v>60000</v>
@@ -1115,13 +1115,13 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="55"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
@@ -1130,9 +1130,9 @@
       <c r="C10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="64"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="19">
         <f>SUM(G11:G13)</f>
         <v>90000</v>
@@ -1205,13 +1205,13 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="61"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
@@ -1220,9 +1220,9 @@
       <c r="C15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
       <c r="G15" s="19">
         <f>SUM(G16:G19)</f>
         <v>153000</v>
@@ -1319,12 +1319,12 @@
     </row>
     <row r="20" spans="2:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="31"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="2:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
@@ -1333,9 +1333,9 @@
       <c r="C21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="21">
         <f>SUM(G22:G26)</f>
         <v>179000</v>
@@ -1452,13 +1452,13 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="58"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
     </row>
     <row r="28" spans="2:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="8" t="s">
@@ -1467,9 +1467,9 @@
       <c r="C28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="21">
         <f>SUM(G29:G32)</f>
         <v>54000</v>
@@ -1565,13 +1565,13 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="56"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="58"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
     </row>
     <row r="34" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="8" t="s">
@@ -1580,9 +1580,9 @@
       <c r="C34" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="61"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="60"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="21">
         <f>SUM(G35:G41)</f>
         <v>126000</v>
@@ -1744,36 +1744,36 @@
       </c>
     </row>
     <row r="42" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="56"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="58"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
     </row>
     <row r="43" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="35"/>
-      <c r="C43" s="35" t="s">
+      <c r="B43" s="57"/>
+      <c r="C43" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="39">
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="61">
         <f>SUM(G7,G10,G15,G21,G28,G34,)</f>
         <v>662000</v>
       </c>
-      <c r="H43" s="40"/>
+      <c r="H43" s="62"/>
     </row>
     <row r="44" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="42"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="64"/>
     </row>
     <row r="45" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H45" s="16"/>
@@ -1782,70 +1782,70 @@
       <c r="H46" s="16"/>
     </row>
     <row r="47" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
     </row>
     <row r="48" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
       <c r="I48" s="16"/>
     </row>
     <row r="49" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="38">
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="60">
         <f>G43</f>
         <v>662000</v>
       </c>
-      <c r="G49" s="38"/>
+      <c r="G49" s="60"/>
       <c r="I49" s="16"/>
     </row>
     <row r="50" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
     </row>
     <row r="51" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
     </row>
     <row r="52" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
     </row>
     <row r="53" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
       <c r="E54" s="1" t="s">
         <v>33</v>
       </c>
@@ -1989,6 +1989,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:F44"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B47:G48"/>
+    <mergeCell ref="B49:E50"/>
+    <mergeCell ref="F49:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="G43:H44"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="B33:H33"/>
@@ -2001,26 +2021,6 @@
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:F44"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B47:G48"/>
-    <mergeCell ref="B49:E50"/>
-    <mergeCell ref="F49:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="G43:H44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>